<commit_message>
Clean up code warnings
Signed-off-by: Dave J Schoepel <dave@theschoepels.com>
</commit_message>
<xml_diff>
--- a/bundles/org.openhab.binding.nadavr/doc/NAT T778 RS232 Commands.xlsx
+++ b/bundles/org.openhab.binding.nadavr/doc/NAT T778 RS232 Commands.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dscho\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Openhab 4.0 - NAD\openhab-addons\bundles\org.openhab.binding.nadavr\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D9F6AD92-AC0B-4BC7-805F-E4E6EA7400BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78D84A9E-07EF-4294-8A21-BCEFE90AA247}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1410" yWindow="1380" windowWidth="20325" windowHeight="12570" xr2:uid="{12A2480B-4871-4070-9326-930EE2AAFD39}"/>
+    <workbookView xWindow="3255" yWindow="1560" windowWidth="20475" windowHeight="12855" xr2:uid="{12A2480B-4871-4070-9326-930EE2AAFD39}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2642,7 +2642,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D3E6324-C926-4746-8672-030C9763D382}">
   <dimension ref="B1:C688"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A667" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G681" sqref="G681"/>
     </sheetView>
   </sheetViews>
@@ -8159,6 +8159,10 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <headerFooter>
+    <oddHeader>&amp;CNAD T-778 RS232 Commands</oddHeader>
+    <oddFooter>Page &amp;P of &amp;N</oddFooter>
+  </headerFooter>
   <tableParts count="1">
     <tablePart r:id="rId2"/>
   </tableParts>

</xml_diff>

<commit_message>
Add T-787 to supported AVRs
Signed-off-by: Dave J Schoepel <dave@theschoepels.com>
</commit_message>
<xml_diff>
--- a/bundles/org.openhab.binding.nadavr/doc/NAT T778 RS232 Commands.xlsx
+++ b/bundles/org.openhab.binding.nadavr/doc/NAT T778 RS232 Commands.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dscho\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Openhab 4.0 - NAD\openhab-addons\bundles\org.openhab.binding.nadavr\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D9F6AD92-AC0B-4BC7-805F-E4E6EA7400BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78D84A9E-07EF-4294-8A21-BCEFE90AA247}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1410" yWindow="1380" windowWidth="20325" windowHeight="12570" xr2:uid="{12A2480B-4871-4070-9326-930EE2AAFD39}"/>
+    <workbookView xWindow="3255" yWindow="1560" windowWidth="20475" windowHeight="12855" xr2:uid="{12A2480B-4871-4070-9326-930EE2AAFD39}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2642,7 +2642,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D3E6324-C926-4746-8672-030C9763D382}">
   <dimension ref="B1:C688"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A667" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G681" sqref="G681"/>
     </sheetView>
   </sheetViews>
@@ -8159,6 +8159,10 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <headerFooter>
+    <oddHeader>&amp;CNAD T-778 RS232 Commands</oddHeader>
+    <oddFooter>Page &amp;P of &amp;N</oddFooter>
+  </headerFooter>
   <tableParts count="1">
     <tablePart r:id="rId2"/>
   </tableParts>

</xml_diff>